<commit_message>
chore: Update source Excel file with CRU-L4 to MIC-L5 fix (#29)
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
Co-Authored-By: Drew Norman <drew.norman@peacefroggaming.com>
</commit_message>
<xml_diff>
--- a/ref data/Band Jump Distances.xlsx
+++ b/ref data/Band Jump Distances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/edf5e7ceff0f2763/Documents/Business/PeaceFrog Gaming/Applications/Band Hopper/ref data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F333739D-AEB4-4BAF-9D1C-43B541434F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{325F76CD-33A9-4DBB-BA96-8268FE988D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="5715" windowWidth="28800" windowHeight="15885" xr2:uid="{E12DAEF5-95D6-472C-891D-D6469350F8D5}"/>
+    <workbookView xWindow="38400" yWindow="5715" windowWidth="28800" windowHeight="15885" activeTab="1" xr2:uid="{E12DAEF5-95D6-472C-891D-D6469350F8D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Route Exists" sheetId="1" r:id="rId1"/>
@@ -279,10 +279,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -604,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390FBEBF-CF8F-4867-BC52-EE44196E11B0}">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="J4" sqref="J4"/>
     </sheetView>
@@ -1641,8 +1637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5BB9FF-BDEE-4B43-B7D2-088EA4348EF3}">
   <dimension ref="B1:X83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,7 +1773,7 @@
         <v>176976</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="P2:W2" si="0">ABS(I2-H2)</f>
+        <f t="shared" ref="S2:V2" si="0">ABS(I2-H2)</f>
         <v>175351</v>
       </c>
       <c r="T2">
@@ -4683,34 +4679,34 @@
         <v>13</v>
       </c>
       <c r="D41" s="1">
-        <v>25688478</v>
+        <v>27667983</v>
       </c>
       <c r="E41" s="1">
-        <v>25917214</v>
+        <v>27439247</v>
       </c>
       <c r="F41" s="1">
-        <v>26120249</v>
+        <v>27236213</v>
       </c>
       <c r="G41" s="1">
-        <v>26397447</v>
+        <v>26959015</v>
       </c>
       <c r="H41" s="1">
-        <v>26589888</v>
+        <v>26766574</v>
       </c>
       <c r="I41" s="1">
-        <v>26805213</v>
+        <v>26551248</v>
       </c>
       <c r="J41" s="1">
-        <v>27076738</v>
+        <v>26279724</v>
       </c>
       <c r="K41" s="1">
-        <v>27384314</v>
+        <v>25972148</v>
       </c>
       <c r="L41" s="1">
-        <v>27662684</v>
+        <v>25693778</v>
       </c>
       <c r="M41" s="1">
-        <v>27835342</v>
+        <v>25521120</v>
       </c>
       <c r="O41">
         <f t="shared" si="1"/>
@@ -4718,7 +4714,7 @@
       </c>
       <c r="P41">
         <f t="shared" si="2"/>
-        <v>203035</v>
+        <v>203034</v>
       </c>
       <c r="Q41">
         <f t="shared" si="3"/>
@@ -4730,11 +4726,11 @@
       </c>
       <c r="S41">
         <f t="shared" si="5"/>
-        <v>215325</v>
+        <v>215326</v>
       </c>
       <c r="T41">
         <f t="shared" si="6"/>
-        <v>271525</v>
+        <v>271524</v>
       </c>
       <c r="U41">
         <f t="shared" si="7"/>

</xml_diff>